<commit_message>
Edited MINSYST Goals.xlsx to update more about plans
</commit_message>
<xml_diff>
--- a/MINSYST Goals.xlsx
+++ b/MINSYST Goals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19200" windowHeight="12180" tabRatio="649" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19200" windowHeight="12180" tabRatio="649" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MINSYST Research Group Plans" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t xml:space="preserve">March </t>
   </si>
@@ -168,6 +168,27 @@
   </si>
   <si>
     <t>Sets</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Erika</t>
+  </si>
+  <si>
+    <t>Thom</t>
+  </si>
+  <si>
+    <t>Koko</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Gino</t>
+  </si>
+  <si>
+    <t>Jestine</t>
   </si>
 </sst>
 </file>
@@ -298,9 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,6 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,11 +739,11 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1312,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,92 +1346,100 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1444,55 +1473,61 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="B17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1504,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,260 +1549,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="9">
         <v>23</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="10">
+      <c r="A2" s="5"/>
+      <c r="B2" s="9">
         <v>24</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10">
+      <c r="A3" s="5"/>
+      <c r="B3" s="9">
         <v>25</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10">
+      <c r="A4" s="5"/>
+      <c r="B4" s="9">
         <v>26</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="10">
+      <c r="A5" s="5"/>
+      <c r="B5" s="9">
         <v>27</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="10">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9">
         <v>28</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="8"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the findings of the Focus Group team.
</commit_message>
<xml_diff>
--- a/MINSYST Goals.xlsx
+++ b/MINSYST Goals.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Z MINSYST - TENTREP\minsyst-research\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19200" windowHeight="12180" tabRatio="649" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19200" windowHeight="11760" tabRatio="649" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MINSYST Research Group Plans" sheetId="1" r:id="rId1"/>
@@ -17,9 +12,9 @@
     <sheet name="Groups Consulation" sheetId="3" r:id="rId3"/>
     <sheet name="Survey" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t xml:space="preserve">March </t>
   </si>
@@ -189,13 +184,34 @@
   </si>
   <si>
     <t>Jestine</t>
+  </si>
+  <si>
+    <t>*What do developers prioritize in developing apps, the users or their personal preference?</t>
+  </si>
+  <si>
+    <t>*What motivates the developers in creating a mobile app?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Find out which is more prefered by the developers mobile or web? </t>
+  </si>
+  <si>
+    <t>The developers main concern is their clients and their user experience.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In terms of their own preference, the students mostly prefer web. Most of the other answers from the professionals are not definite and it usually depends on the given  situation like if security is prioritized, web is prefered. </t>
+  </si>
+  <si>
+    <t>DESIGN TEAM RESEARCH: In designing mobile apps, the preferences / professional opinion of various designers may differ, however the customer (target market, users)’s requirements should be taken into consideration</t>
+  </si>
+  <si>
+    <t>Improvement of the society and how they can help in providing solutions to the users.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,14 +329,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -328,9 +343,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +456,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -604,27 +633,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:E12"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -638,7 +667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -650,7 +679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
@@ -660,7 +689,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -670,7 +699,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -682,7 +711,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -694,7 +723,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -704,10 +733,10 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
@@ -716,14 +745,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
@@ -733,19 +762,19 @@
     <col min="8" max="8" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -771,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -781,7 +810,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -791,7 +820,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -801,7 +830,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -811,7 +840,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -821,7 +850,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -831,7 +860,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -841,7 +870,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -851,7 +880,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -861,7 +890,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -871,7 +900,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -881,7 +910,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -891,7 +920,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -901,7 +930,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -911,7 +940,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -921,7 +950,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -931,7 +960,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -941,7 +970,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -951,7 +980,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -961,7 +990,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -971,7 +1000,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -981,7 +1010,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -991,7 +1020,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1001,7 +1030,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1011,7 +1040,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1021,7 +1050,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1031,7 +1060,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1041,7 +1070,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1051,7 +1080,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1061,7 +1090,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1071,7 +1100,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1081,7 +1110,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1091,7 +1120,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1101,7 +1130,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1111,7 +1140,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1121,7 +1150,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1131,7 +1160,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1141,7 +1170,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1151,7 +1180,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1161,7 +1190,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1171,7 +1200,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1181,7 +1210,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1191,7 +1220,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1201,7 +1230,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1211,7 +1240,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1221,7 +1250,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1231,7 +1260,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1241,7 +1270,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1251,7 +1280,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1261,7 +1290,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1271,7 +1300,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1281,7 +1310,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1291,7 +1320,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1301,7 +1330,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1311,7 +1340,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1330,22 +1359,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="14" t="s">
         <v>40</v>
       </c>
@@ -1362,172 +1393,186 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" ht="81" customHeight="1">
+      <c r="A17" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12" t="s">
+      <c r="C17" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" ht="147" customHeight="1">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12" t="s">
+      <c r="C18" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45.75" customHeight="1">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="C19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1536,273 +1581,273 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="8">
         <v>23</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="5"/>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>24</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="5"/>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>25</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="5"/>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>26</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="5"/>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>27</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="5"/>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:5">
+      <c r="B9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:5">
+      <c r="B10" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="7"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="7"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="7"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="7"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="7"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="7"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="7"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="7"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="7"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="7"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="7"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="7"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="7"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="7"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="7"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="7"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="7"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="7"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="7"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="7"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="7"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="7"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="7"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="7"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="7"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="7"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="7"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="7"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added status report for Minsyst
</commit_message>
<xml_diff>
--- a/MINSYST Goals.xlsx
+++ b/MINSYST Goals.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Z MINSYST - TENTREP\minsyst-research\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19200" windowHeight="11760" tabRatio="649" activeTab="2"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19200" windowHeight="11760" tabRatio="649"/>
   </bookViews>
   <sheets>
     <sheet name="MINSYST Research Group Plans" sheetId="1" r:id="rId1"/>
@@ -13,8 +18,8 @@
     <sheet name="Survey" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t xml:space="preserve">March </t>
   </si>
@@ -241,13 +246,25 @@
   </si>
   <si>
     <t>Both developer and user have some things to be taken in consideration. For instance, for the developer's side, the industry has its own implications in a mobile application. For the users, the purpose of the application is vital.</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +354,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -402,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -443,6 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,27 +739,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E12"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -749,7 +787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -761,7 +799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
@@ -771,7 +809,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -781,7 +819,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -793,7 +831,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -805,7 +843,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -815,10 +853,10 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
@@ -827,14 +865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
@@ -844,7 +882,7 @@
     <col min="8" max="8" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -856,7 +894,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -882,7 +920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -892,7 +930,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -902,7 +940,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -912,7 +950,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -922,7 +960,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -932,7 +970,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -942,7 +980,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -952,7 +990,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -962,7 +1000,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -972,7 +1010,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -982,7 +1020,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -992,7 +1030,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1002,7 +1040,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1012,7 +1050,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1022,7 +1060,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1032,7 +1070,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1042,7 +1080,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1052,7 +1090,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1062,7 +1100,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1072,7 +1110,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1082,7 +1120,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1092,7 +1130,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1102,7 +1140,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1112,7 +1150,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1122,7 +1160,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1132,7 +1170,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1142,7 +1180,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1152,7 +1190,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1162,7 +1200,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1172,7 +1210,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1182,7 +1220,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1192,7 +1230,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1202,7 +1240,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1212,7 +1250,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1222,7 +1260,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1232,7 +1270,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1242,7 +1280,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1252,7 +1290,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1262,7 +1300,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1272,7 +1310,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1282,7 +1320,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1292,7 +1330,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1302,7 +1340,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1312,7 +1350,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1322,7 +1360,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1332,7 +1370,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1342,7 +1380,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1352,7 +1390,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1362,7 +1400,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1372,7 +1410,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1382,7 +1420,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1392,7 +1430,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1402,7 +1440,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1412,7 +1450,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1422,7 +1460,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1441,14 +1479,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="17" bestFit="1" customWidth="1"/>
@@ -1458,7 +1496,7 @@
     <col min="6" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>40</v>
       </c>
@@ -1475,7 +1513,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
@@ -1486,49 +1524,49 @@
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>39</v>
       </c>
@@ -1545,7 +1583,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="15" t="s">
         <v>52</v>
@@ -1558,7 +1596,7 @@
       </c>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="15" t="s">
         <v>53</v>
@@ -1571,7 +1609,7 @@
       </c>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15" t="s">
@@ -1582,7 +1620,7 @@
       </c>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15" t="s">
@@ -1593,7 +1631,7 @@
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
@@ -1602,28 +1640,28 @@
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="1:5" ht="81" customHeight="1">
+    <row r="19" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>38</v>
       </c>
@@ -1638,7 +1676,7 @@
       </c>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" ht="147" customHeight="1">
+    <row r="20" spans="1:5" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="16" t="s">
         <v>49</v>
@@ -1653,7 +1691,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45.75" customHeight="1">
+    <row r="21" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>50</v>
@@ -1666,28 +1704,28 @@
       </c>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1704,19 +1742,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +1765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="8">
         <v>24</v>
@@ -1736,7 +1774,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="8">
         <v>25</v>
@@ -1745,7 +1783,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="8">
         <v>26</v>
@@ -1754,7 +1792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="8">
         <v>27</v>
@@ -1763,7 +1801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="8">
         <v>28</v>
@@ -1772,7 +1810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>46</v>
       </c>
@@ -1786,7 +1824,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>32</v>
       </c>
@@ -1794,61 +1832,61 @@
       <c r="D10" s="11"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="3"/>
       <c r="D11" s="11"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="3"/>
       <c r="D13" s="11"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="3"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="3"/>
       <c r="D15" s="11"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="3"/>
       <c r="D16" s="11"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="3"/>
       <c r="D17" s="11"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="3"/>
       <c r="D18" s="11"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="3"/>
       <c r="D19" s="11"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>33</v>
       </c>
@@ -1856,61 +1894,61 @@
       <c r="D20" s="11"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="10"/>
       <c r="D26" s="11"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
@@ -1918,55 +1956,55 @@
       <c r="D30" s="11"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="11"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="11"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="5"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="11"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="11"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="11"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="11"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="11"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="11"/>

</xml_diff>